<commit_message>
back-end no write to json
</commit_message>
<xml_diff>
--- a/uploads/invoices.xlsx
+++ b/uploads/invoices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,204 +436,139 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>AFM_issuer</t>
+          <t>MARK</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name_issuer</t>
+          <t>ΑΦΜ</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>Επωνυμία</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>classification</t>
+          <t>Σειρά</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>issueDate</t>
+          <t>Αριθμός</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>mark</t>
+          <t>Ημερομηνία</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>series</t>
+          <t>Είδος</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>totalNetValue</t>
+          <t>ΦΠΑ_ΚΑΤΗΓΟΡΙΑ</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>totalVatAmount</t>
+          <t>Καθαρή Αξία</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>vatCategory</t>
+          <t>ΦΠΑ</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Σύνολο</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>094439854</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>7061</t>
-        </is>
-      </c>
+          <t>400008186167654</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>χαρακτηρισμενο</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
+          <t>8Μ0ΤΔΑ</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>400010783401151</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>11Μ0ΤΔΑ</t>
-        </is>
-      </c>
+          <t>2025-01-03</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>37.01</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>8.88</t>
+          <t>75.98</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>18.24</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>94.22</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>094439854</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3669</t>
-        </is>
-      </c>
+          <t>400008186167654</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>χαρακτηρισμενο</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2025-05-12</t>
-        </is>
-      </c>
+          <t>8Μ0ΤΔΑ</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>400009406874951</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>8Μ0ΤΔΑ</t>
-        </is>
-      </c>
+          <t>2025-01-03</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>172.8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>41.47</t>
+          <t>75.98</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>094439854</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3669</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>χαρακτηρισμενο</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2025-05-12</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>400009406874951</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>8Μ0ΤΔΑ</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>172.8</v>
-      </c>
-      <c r="I4" t="n">
-        <v>41.47</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>18.24</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>94.22</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
inv type 1st try
</commit_message>
<xml_diff>
--- a/uploads/invoices.xlsx
+++ b/uploads/invoices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,11 @@
           <t>Σύνολο</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Χαρακτηρισμός</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -530,11 +535,12 @@
           <t>94.22</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>400008186167654</t>
+          <t>400008207899445</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -547,7 +553,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-01-03</t>
+          <t>2025-01-07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -558,19 +564,104 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>75.98</t>
+          <t>70.03</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>18.24</t>
+          <t>16.81</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>94.22</t>
-        </is>
-      </c>
+          <t>86.84</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>400008195607600</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8Μ0ΤΔΑ</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-01-04</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>34.34</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>8.24</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>42.58</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>400008429648898</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>8Μ0ΤΔΑ</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-01-29</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>146.07</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>35.06</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>181.13</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
only a/amissing from modal, fix list next
</commit_message>
<xml_diff>
--- a/uploads/invoices.xlsx
+++ b/uploads/invoices.xlsx
@@ -501,13 +501,17 @@
           <t>400008186167654</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>8Μ0ΤΔΑ</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>094439854</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ΤΡΑΚΑΔΑΣ Α.Ε.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
@@ -515,11 +519,7 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>75.98</t>
@@ -540,7 +540,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>400008186167654</t>
+          <t>400008195607600</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -557,24 +557,24 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-01-03</t>
+          <t>2025-01-04</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>75.98</t>
+          <t>34.34</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>18.24</t>
+          <t>8.24</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>94.22</t>
+          <t>42.58</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>

</xml_diff>